<commit_message>
Adding chapter 5 content
</commit_message>
<xml_diff>
--- a/17. LinkedIn Learning/01. Microsoft Excel/01. Master Microsoft Excel - Learning Path/02. Excel - Advanced Formulas and Functions/Material/Ex_Files_Excel_Advanced_Formulas_Functions/Exercise Files/Ch-5/5-Stat.xlsx
+++ b/17. LinkedIn Learning/01. Microsoft Excel/01. Master Microsoft Excel - Learning Path/02. Excel - Advanced Formulas and Functions/Material/Ex_Files_Excel_Advanced_Formulas_Functions/Exercise Files/Ch-5/5-Stat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Descargas\1. GIT\OnlineCourses\17. LinkedIn Learning\01. Microsoft Excel\01. Master Microsoft Excel - Learning Path\02. Excel - Advanced Formulas and Functions\Material\Ex_Files_Excel_Advanced_Formulas_Functions\Exercise Files\Ch-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D1C1EB-B0D7-4D13-9C7E-A1695E73913F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D491BB-36C2-4E87-A728-7508D43EBC1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDIAN MODE" sheetId="5" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3117" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3125" uniqueCount="840">
   <si>
     <t>Hire Date</t>
   </si>
@@ -2561,6 +2561,30 @@
   </si>
   <si>
     <t>Acosta, Daniel</t>
+  </si>
+  <si>
+    <t>Second highest value</t>
+  </si>
+  <si>
+    <t>Third highest value</t>
+  </si>
+  <si>
+    <t>Fourth highest value</t>
+  </si>
+  <si>
+    <t>5th highest value</t>
+  </si>
+  <si>
+    <t>Using Max (Highest value)</t>
+  </si>
+  <si>
+    <t>Using Large (Highest value)</t>
+  </si>
+  <si>
+    <t>Numerical values</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -2667,7 +2691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2705,6 +2729,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2715,7 +2752,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2794,9 +2831,6 @@
     <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2806,9 +2840,16 @@
     </xf>
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -2819,7 +2860,207 @@
     <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="22"/>
+        </left>
+        <right style="thin">
+          <color indexed="22"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="22"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="22"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2835,6 +3076,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D46FB47-3DD1-4B06-9434-97E63E8D16B4}" name="Tabla1" displayName="Tabla1" ref="A1:G100" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10" headerRowCellStyle="Normal 2" dataCellStyle="Comma 2">
+  <autoFilter ref="A1:G100" xr:uid="{F17252EE-5BFE-4793-9FCA-3B1C9A0310D5}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{239423F0-C8A1-4112-91F6-EF15D03394D2}" name="Employee Name" dataDxfId="8" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{81084E3C-F6EB-4B05-8170-02D0C020D046}" name="Hire Date" dataDxfId="7" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{F946C489-6CFA-4BD6-887C-5C7645A20CAE}" name="Years" dataDxfId="6" dataCellStyle="Comma 2">
+      <calculatedColumnFormula>DATEDIF(B2,TODAY(),"Y")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{536A6833-6602-4C16-BEED-4E8FC6D8A30F}" name="Salary" dataDxfId="5" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9559D23A-4B99-4104-A5AE-D19DBAF84765}" name="Rank" dataDxfId="4" dataCellStyle="Comma 2">
+      <calculatedColumnFormula>RANK(D2,D:D)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5C39ED5C-8E59-4919-84F8-528E0D8431C5}" name="Benefits" dataDxfId="3" dataCellStyle="Comma 2"/>
+    <tableColumn id="7" xr3:uid="{30536CAF-E1DC-4D22-B68F-6F2C579B3A39}" name="Job Rating" dataDxfId="2" dataCellStyle="Normal 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3164,7 +3425,9 @@
   </sheetPr>
   <dimension ref="A1:AA742"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3252,7 +3515,10 @@
       <c r="H2" s="22">
         <v>2</v>
       </c>
-      <c r="J2" s="13"/>
+      <c r="J2" s="13">
+        <f>AVERAGE(G:G)</f>
+        <v>64680.66801619433</v>
+      </c>
       <c r="M2" s="10" t="s">
         <v>18</v>
       </c>
@@ -3344,6 +3610,10 @@
       <c r="H4" s="22">
         <v>1</v>
       </c>
+      <c r="J4" s="13">
+        <f>MEDIAN(G:G)</f>
+        <v>61718</v>
+      </c>
       <c r="M4" s="10" t="s">
         <v>22</v>
       </c>
@@ -3434,6 +3704,10 @@
       <c r="H6" s="22">
         <v>5</v>
       </c>
+      <c r="J6" s="9">
+        <f>MODE(E:E)</f>
+        <v>3</v>
+      </c>
       <c r="M6" s="10" t="s">
         <v>26</v>
       </c>
@@ -3480,6 +3754,10 @@
       <c r="H7" s="22">
         <v>4</v>
       </c>
+      <c r="J7" s="9">
+        <f>MODE(H:H)</f>
+        <v>5</v>
+      </c>
       <c r="L7" s="13"/>
       <c r="M7" s="10" t="s">
         <v>28</v>
@@ -3804,23 +4082,23 @@
       <c r="M14" s="9" t="s">
         <v>815</v>
       </c>
-      <c r="N14" s="44">
+      <c r="N14" s="43">
         <f>AVERAGE(N2:N13)</f>
         <v>582.25</v>
       </c>
-      <c r="O14" s="44">
+      <c r="O14" s="43">
         <f t="shared" ref="O14:R14" si="1">AVERAGE(O2:O13)</f>
         <v>582.25</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="43">
         <f t="shared" si="1"/>
         <v>566</v>
       </c>
-      <c r="Q14" s="44">
+      <c r="Q14" s="43">
         <f t="shared" si="1"/>
         <v>574.33333333333337</v>
       </c>
-      <c r="R14" s="44">
+      <c r="R14" s="43">
         <f t="shared" si="1"/>
         <v>598.08333333333337</v>
       </c>
@@ -3838,7 +4116,7 @@
       </c>
       <c r="D15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="22">
         <v>0</v>
@@ -3855,23 +4133,23 @@
       <c r="M15" s="9" t="s">
         <v>816</v>
       </c>
-      <c r="N15" s="44">
+      <c r="N15" s="43">
         <f>MEDIAN(N2:N13)</f>
         <v>479.5</v>
       </c>
-      <c r="O15" s="44">
+      <c r="O15" s="43">
         <f t="shared" ref="O15:R15" si="2">MEDIAN(O2:O13)</f>
         <v>514.5</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="43">
         <f t="shared" si="2"/>
         <v>505</v>
       </c>
-      <c r="Q15" s="44">
+      <c r="Q15" s="43">
         <f t="shared" si="2"/>
         <v>494</v>
       </c>
-      <c r="R15" s="44">
+      <c r="R15" s="43">
         <f t="shared" si="2"/>
         <v>533</v>
       </c>
@@ -3903,11 +4181,11 @@
       <c r="H16" s="22">
         <v>5</v>
       </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -11099,7 +11377,7 @@
       </c>
       <c r="D290" s="12">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E290" s="22">
         <v>5</v>
@@ -12367,7 +12645,7 @@
       </c>
       <c r="D338" s="12">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E338" s="22">
         <v>3</v>
@@ -21940,7 +22218,7 @@
       </c>
       <c r="D701" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E701" s="22">
         <v>1</v>
@@ -23045,7 +23323,9 @@
   </sheetPr>
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23064,7 +23344,7 @@
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -23091,14 +23371,25 @@
       <c r="B2" s="12">
         <v>111686</v>
       </c>
+      <c r="C2" s="7">
+        <f>RANK(B2,B:B,1)</f>
+        <v>36</v>
+      </c>
       <c r="D2" s="32"/>
       <c r="F2" s="18">
-        <v>43497</v>
+        <v>43500</v>
       </c>
       <c r="G2" s="5">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="H2" s="7">
+        <f>RANK(G2,G:G)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <f>_xlfn.RANK.AVG(G2,G:G)</f>
+        <v>1</v>
+      </c>
       <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -23108,14 +23399,25 @@
       <c r="B3" s="12">
         <v>121604</v>
       </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C45" si="0">RANK(B3,B:B,1)</f>
+        <v>43</v>
+      </c>
       <c r="D3" s="32"/>
       <c r="F3" s="18">
-        <v>43500</v>
+        <v>43508</v>
       </c>
       <c r="G3" s="5">
-        <v>29</v>
-      </c>
-      <c r="H3" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="H3" s="7">
+        <f>RANK(G3,G:G)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="4">
+        <f>_xlfn.RANK.AVG(G3,G:G)</f>
+        <v>2.5</v>
+      </c>
       <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -23125,14 +23427,25 @@
       <c r="B4" s="12">
         <v>75799</v>
       </c>
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="D4" s="32"/>
       <c r="F4" s="18">
-        <v>43501</v>
+        <v>43517</v>
       </c>
       <c r="G4" s="5">
-        <v>13</v>
-      </c>
-      <c r="H4" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="H4" s="7">
+        <f>RANK(G4,G:G)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <f>_xlfn.RANK.AVG(G4,G:G)</f>
+        <v>2.5</v>
+      </c>
       <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -23142,14 +23455,25 @@
       <c r="B5" s="12">
         <v>74304</v>
       </c>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="D5" s="32"/>
       <c r="F5" s="18">
-        <v>43502</v>
+        <v>43497</v>
       </c>
       <c r="G5" s="5">
-        <v>21</v>
-      </c>
-      <c r="H5" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="H5" s="7">
+        <f>RANK(G5,G:G)</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="4">
+        <f>_xlfn.RANK.AVG(G5,G:G)</f>
+        <v>5</v>
+      </c>
       <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -23159,14 +23483,25 @@
       <c r="B6" s="12">
         <v>111686</v>
       </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="D6" s="32"/>
       <c r="F6" s="18">
-        <v>43503</v>
+        <v>43518</v>
       </c>
       <c r="G6" s="5">
-        <v>19</v>
-      </c>
-      <c r="H6" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="H6" s="7">
+        <f>RANK(G6,G:G)</f>
+        <v>4</v>
+      </c>
+      <c r="I6" s="4">
+        <f>_xlfn.RANK.AVG(G6,G:G)</f>
+        <v>5</v>
+      </c>
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -23176,14 +23511,25 @@
       <c r="B7" s="12">
         <v>101365</v>
       </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="D7" s="32"/>
       <c r="F7" s="18">
-        <v>43504</v>
+        <v>43523</v>
       </c>
       <c r="G7" s="5">
-        <v>7</v>
-      </c>
-      <c r="H7" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="H7" s="7">
+        <f>RANK(G7,G:G)</f>
+        <v>4</v>
+      </c>
+      <c r="I7" s="4">
+        <f>_xlfn.RANK.AVG(G7,G:G)</f>
+        <v>5</v>
+      </c>
       <c r="J7" s="31"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -23193,14 +23539,25 @@
       <c r="B8" s="12">
         <v>119001</v>
       </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="D8" s="32"/>
       <c r="F8" s="18">
-        <v>43507</v>
+        <v>43522</v>
       </c>
       <c r="G8" s="5">
-        <v>11</v>
-      </c>
-      <c r="H8" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="H8" s="7">
+        <f>RANK(G8,G:G)</f>
+        <v>7</v>
+      </c>
+      <c r="I8" s="4">
+        <f>_xlfn.RANK.AVG(G8,G:G)</f>
+        <v>7</v>
+      </c>
       <c r="J8" s="31"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -23210,14 +23567,25 @@
       <c r="B9" s="12">
         <v>73102</v>
       </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="D9" s="32"/>
       <c r="F9" s="18">
-        <v>43508</v>
+        <v>43502</v>
       </c>
       <c r="G9" s="5">
-        <v>27</v>
-      </c>
-      <c r="H9" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="H9" s="7">
+        <f>RANK(G9,G:G)</f>
+        <v>8</v>
+      </c>
+      <c r="I9" s="4">
+        <f>_xlfn.RANK.AVG(G9,G:G)</f>
+        <v>8.5</v>
+      </c>
       <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -23227,14 +23595,25 @@
       <c r="B10" s="12">
         <v>79262</v>
       </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="D10" s="32"/>
       <c r="F10" s="18">
-        <v>43509</v>
+        <v>43521</v>
       </c>
       <c r="G10" s="5">
-        <v>11</v>
-      </c>
-      <c r="H10" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="H10" s="7">
+        <f>RANK(G10,G:G)</f>
+        <v>8</v>
+      </c>
+      <c r="I10" s="4">
+        <f>_xlfn.RANK.AVG(G10,G:G)</f>
+        <v>8.5</v>
+      </c>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -23244,14 +23623,25 @@
       <c r="B11" s="12">
         <v>74666</v>
       </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="D11" s="32"/>
       <c r="F11" s="18">
-        <v>43510</v>
+        <v>43503</v>
       </c>
       <c r="G11" s="5">
-        <v>7</v>
-      </c>
-      <c r="H11" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="H11" s="7">
+        <f>RANK(G11,G:G)</f>
+        <v>10</v>
+      </c>
+      <c r="I11" s="4">
+        <f>_xlfn.RANK.AVG(G11,G:G)</f>
+        <v>11</v>
+      </c>
       <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -23261,6 +23651,10 @@
       <c r="B12" s="12">
         <v>68347</v>
       </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="D12" s="32"/>
       <c r="F12" s="18">
         <v>43511</v>
@@ -23268,7 +23662,14 @@
       <c r="G12" s="5">
         <v>19</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7">
+        <f>RANK(G12,G:G)</f>
+        <v>10</v>
+      </c>
+      <c r="I12" s="4">
+        <f>_xlfn.RANK.AVG(G12,G:G)</f>
+        <v>11</v>
+      </c>
       <c r="J12" s="31"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -23278,14 +23679,25 @@
       <c r="B13" s="12">
         <v>78409</v>
       </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="D13" s="32"/>
       <c r="F13" s="18">
-        <v>43514</v>
+        <v>43524</v>
       </c>
       <c r="G13" s="5">
+        <v>19</v>
+      </c>
+      <c r="H13" s="7">
+        <f>RANK(G13,G:G)</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="4">
+        <f>_xlfn.RANK.AVG(G13,G:G)</f>
         <v>11</v>
       </c>
-      <c r="H13" s="7"/>
       <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -23295,14 +23707,25 @@
       <c r="B14" s="12">
         <v>110448</v>
       </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="D14" s="32"/>
       <c r="F14" s="18">
-        <v>43515</v>
+        <v>43501</v>
       </c>
       <c r="G14" s="5">
-        <v>5</v>
-      </c>
-      <c r="H14" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="H14" s="7">
+        <f>RANK(G14,G:G)</f>
+        <v>13</v>
+      </c>
+      <c r="I14" s="4">
+        <f>_xlfn.RANK.AVG(G14,G:G)</f>
+        <v>13</v>
+      </c>
       <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -23312,14 +23735,25 @@
       <c r="B15" s="12">
         <v>110203</v>
       </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
       <c r="D15" s="32"/>
       <c r="F15" s="18">
-        <v>43516</v>
+        <v>43507</v>
       </c>
       <c r="G15" s="5">
-        <v>9</v>
-      </c>
-      <c r="H15" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="H15" s="7">
+        <f>RANK(G15,G:G)</f>
+        <v>14</v>
+      </c>
+      <c r="I15" s="4">
+        <f>_xlfn.RANK.AVG(G15,G:G)</f>
+        <v>15</v>
+      </c>
       <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -23329,14 +23763,25 @@
       <c r="B16" s="12">
         <v>101128</v>
       </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
       <c r="D16" s="32"/>
       <c r="F16" s="18">
-        <v>43517</v>
+        <v>43509</v>
       </c>
       <c r="G16" s="5">
-        <v>27</v>
-      </c>
-      <c r="H16" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="H16" s="7">
+        <f>RANK(G16,G:G)</f>
+        <v>14</v>
+      </c>
+      <c r="I16" s="4">
+        <f>_xlfn.RANK.AVG(G16,G:G)</f>
+        <v>15</v>
+      </c>
       <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -23346,14 +23791,25 @@
       <c r="B17" s="12">
         <v>96418</v>
       </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
       <c r="D17" s="32"/>
       <c r="F17" s="18">
-        <v>43518</v>
+        <v>43514</v>
       </c>
       <c r="G17" s="5">
-        <v>25</v>
-      </c>
-      <c r="H17" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="H17" s="7">
+        <f>RANK(G17,G:G)</f>
+        <v>14</v>
+      </c>
+      <c r="I17" s="4">
+        <f>_xlfn.RANK.AVG(G17,G:G)</f>
+        <v>15</v>
+      </c>
       <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -23363,14 +23819,25 @@
       <c r="B18" s="12">
         <v>121308</v>
       </c>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
       <c r="D18" s="32"/>
       <c r="F18" s="18">
-        <v>43521</v>
+        <v>43516</v>
       </c>
       <c r="G18" s="5">
-        <v>21</v>
-      </c>
-      <c r="H18" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="H18" s="7">
+        <f>RANK(G18,G:G)</f>
+        <v>17</v>
+      </c>
+      <c r="I18" s="4">
+        <f>_xlfn.RANK.AVG(G18,G:G)</f>
+        <v>17</v>
+      </c>
       <c r="J18" s="31"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -23380,14 +23847,25 @@
       <c r="B19" s="12">
         <v>80732</v>
       </c>
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="D19" s="32"/>
       <c r="F19" s="18">
-        <v>43522</v>
+        <v>43504</v>
       </c>
       <c r="G19" s="5">
-        <v>23</v>
-      </c>
-      <c r="H19" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="H19" s="7">
+        <f>RANK(G19,G:G)</f>
+        <v>18</v>
+      </c>
+      <c r="I19" s="4">
+        <f>_xlfn.RANK.AVG(G19,G:G)</f>
+        <v>18.5</v>
+      </c>
       <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -23397,14 +23875,25 @@
       <c r="B20" s="12">
         <v>66573</v>
       </c>
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="D20" s="32"/>
       <c r="F20" s="18">
-        <v>43523</v>
+        <v>43510</v>
       </c>
       <c r="G20" s="5">
-        <v>25</v>
-      </c>
-      <c r="H20" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="H20" s="7">
+        <f>RANK(G20,G:G)</f>
+        <v>18</v>
+      </c>
+      <c r="I20" s="4">
+        <f>_xlfn.RANK.AVG(G20,G:G)</f>
+        <v>18.5</v>
+      </c>
       <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -23414,14 +23903,25 @@
       <c r="B21" s="12">
         <v>107695</v>
       </c>
+      <c r="C21" s="7">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
       <c r="D21" s="32"/>
       <c r="F21" s="18">
-        <v>43524</v>
+        <v>43515</v>
       </c>
       <c r="G21" s="5">
-        <v>19</v>
-      </c>
-      <c r="H21" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="H21" s="7">
+        <f>RANK(G21,G:G)</f>
+        <v>20</v>
+      </c>
+      <c r="I21" s="4">
+        <f>_xlfn.RANK.AVG(G21,G:G)</f>
+        <v>20</v>
+      </c>
       <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -23431,6 +23931,10 @@
       <c r="B22" s="12">
         <v>75425</v>
       </c>
+      <c r="C22" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="D22" s="32"/>
       <c r="F22" s="18"/>
     </row>
@@ -23441,6 +23945,10 @@
       <c r="B23" s="12">
         <v>120404</v>
       </c>
+      <c r="C23" s="7">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
       <c r="D23" s="32"/>
       <c r="F23" s="18"/>
     </row>
@@ -23451,6 +23959,10 @@
       <c r="B24" s="12">
         <v>103608</v>
       </c>
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
       <c r="D24" s="32"/>
       <c r="F24" s="18"/>
     </row>
@@ -23461,6 +23973,10 @@
       <c r="B25" s="12">
         <v>103657</v>
       </c>
+      <c r="C25" s="7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="D25" s="32"/>
       <c r="F25" s="18"/>
     </row>
@@ -23471,6 +23987,10 @@
       <c r="B26" s="12">
         <v>103259</v>
       </c>
+      <c r="C26" s="7">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="F26" s="18"/>
     </row>
@@ -23481,6 +24001,10 @@
       <c r="B27" s="12">
         <v>84107</v>
       </c>
+      <c r="C27" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -23490,6 +24014,10 @@
       <c r="B28" s="12">
         <v>101481</v>
       </c>
+      <c r="C28" s="7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -23499,6 +24027,10 @@
       <c r="B29" s="12">
         <v>70695</v>
       </c>
+      <c r="C29" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -23508,6 +24040,10 @@
       <c r="B30" s="12">
         <v>89510</v>
       </c>
+      <c r="C30" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
@@ -23516,6 +24052,10 @@
       <c r="B31" s="12">
         <v>66777</v>
       </c>
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
@@ -23524,114 +24064,170 @@
       <c r="B32" s="12">
         <v>102833</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="7">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>803</v>
       </c>
       <c r="B33" s="12">
         <v>110404</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="12">
         <v>93239</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>348</v>
       </c>
       <c r="B35" s="12">
         <v>103041</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>682</v>
       </c>
       <c r="B36" s="12">
         <v>66579</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B37" s="12">
         <v>110812</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="7">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="12">
         <v>98598</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>315</v>
       </c>
       <c r="B39" s="12">
         <v>90126</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>413</v>
       </c>
       <c r="B40" s="12">
         <v>71445</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B41" s="12">
         <v>83926</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>464</v>
       </c>
       <c r="B42" s="12">
         <v>114408</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" s="7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B43" s="12">
         <v>113020</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" s="7">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>341</v>
       </c>
       <c r="B44" s="12">
         <v>121824</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>217</v>
       </c>
       <c r="B45" s="12">
         <v>70990</v>
       </c>
+      <c r="C45" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C45">
-    <sortCondition ref="A4"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:I21">
+    <sortCondition descending="1" ref="G1:G21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23645,9 +24241,11 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:F742"/>
+  <dimension ref="A1:H742"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23656,20 +24254,23 @@
     <col min="3" max="3" width="12.88671875" style="7" customWidth="1"/>
     <col min="4" max="4" width="7.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="19.88671875" style="4"/>
+    <col min="6" max="6" width="22.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" style="4"/>
+    <col min="8" max="8" width="23.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="19.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>433</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>434</v>
       </c>
@@ -23679,8 +24280,22 @@
       <c r="D2" s="1" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="31">
+        <f>MAX(B:B)</f>
+        <v>151952</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="G2" s="4">
+        <f>LARGE(B:B,1)</f>
+        <v>151952</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>92</v>
       </c>
@@ -23690,8 +24305,15 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="4">
+        <f>LARGE(B:B,D3)</f>
+        <v>151866</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>820</v>
       </c>
@@ -23701,8 +24323,15 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="4">
+        <f t="shared" ref="E4:E6" si="0">LARGE(B:B,D4)</f>
+        <v>150802</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>333</v>
       </c>
@@ -23712,8 +24341,15 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>150614</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>436</v>
       </c>
@@ -23723,8 +24359,15 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>150136</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>355</v>
       </c>
@@ -23733,7 +24376,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>438</v>
       </c>
@@ -23745,7 +24388,7 @@
       </c>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>439</v>
       </c>
@@ -23755,8 +24398,12 @@
       <c r="D9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
+        <f>SMALL(B:B,D9)</f>
+        <v>31577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>819</v>
       </c>
@@ -23766,8 +24413,12 @@
       <c r="D10" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="4">
+        <f t="shared" ref="E10:E12" si="1">SMALL(B:B,D10)</f>
+        <v>31706</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>245</v>
       </c>
@@ -23777,8 +24428,12 @@
       <c r="D11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="4">
+        <f t="shared" si="1"/>
+        <v>31806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
@@ -23788,8 +24443,12 @@
       <c r="D12" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="4">
+        <f t="shared" si="1"/>
+        <v>31835</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>263</v>
       </c>
@@ -23797,7 +24456,7 @@
         <v>34763</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>440</v>
       </c>
@@ -23805,7 +24464,7 @@
         <v>73291</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>817</v>
       </c>
@@ -23813,7 +24472,7 @@
         <v>129562</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>818</v>
       </c>
@@ -29644,17 +30303,19 @@
   </sheetPr>
   <dimension ref="A1:T742"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" style="9" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="9" customWidth="1"/>
     <col min="8" max="10" width="2.6640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="12.109375" style="24" customWidth="1"/>
     <col min="12" max="12" width="36.33203125" style="9" customWidth="1"/>
@@ -29670,26 +30331,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="45" t="s">
         <v>420</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>3</v>
+      <c r="G1" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="24">
+        <v>1048576</v>
       </c>
       <c r="M1" s="19" t="s">
         <v>11</v>
@@ -29727,7 +30391,7 @@
         <f t="shared" ref="C2:C33" ca="1" si="0">DATEDIF(B2,TODAY(),"Y")</f>
         <v>21</v>
       </c>
-      <c r="D2" s="41">
+      <c r="D2" s="40">
         <v>27582</v>
       </c>
       <c r="E2" s="12">
@@ -29740,6 +30404,10 @@
       </c>
       <c r="H2" s="22"/>
       <c r="I2" s="23"/>
+      <c r="K2" s="24">
+        <f>COUNTBLANK(F2:F100)</f>
+        <v>28</v>
+      </c>
       <c r="L2" s="12" t="s">
         <v>808</v>
       </c>
@@ -29777,7 +30445,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="40">
         <v>117406</v>
       </c>
       <c r="E3" s="12">
@@ -29826,7 +30494,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="40">
         <v>35730</v>
       </c>
       <c r="E4" s="12">
@@ -29878,7 +30546,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="40">
         <v>121604</v>
       </c>
       <c r="E5" s="12">
@@ -29931,7 +30599,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="40">
         <v>62768</v>
       </c>
       <c r="E6" s="12">
@@ -29985,7 +30653,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="40">
         <v>29875</v>
       </c>
       <c r="E7" s="12">
@@ -29999,6 +30667,10 @@
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="J7" s="13"/>
+      <c r="K7" s="24">
+        <f>COUNTBLANK(Tabla1[Benefits])</f>
+        <v>28</v>
+      </c>
       <c r="L7" s="12"/>
       <c r="M7" s="9" t="s">
         <v>236</v>
@@ -30034,7 +30706,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="40">
         <v>38841</v>
       </c>
       <c r="E8" s="12">
@@ -30048,7 +30720,10 @@
       <c r="H8" s="22"/>
       <c r="I8" s="23"/>
       <c r="J8" s="13"/>
-      <c r="L8" s="12"/>
+      <c r="L8" s="12">
+        <f>COUNTBLANK(N2:S16)</f>
+        <v>14</v>
+      </c>
       <c r="M8" s="9" t="s">
         <v>154</v>
       </c>
@@ -30086,7 +30761,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="40">
         <v>27136</v>
       </c>
       <c r="E9" s="12">
@@ -30139,7 +30814,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="40">
         <v>75799</v>
       </c>
       <c r="E10" s="12">
@@ -30190,7 +30865,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="40">
         <v>74304</v>
       </c>
       <c r="E11" s="12">
@@ -30240,7 +30915,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="40">
         <v>111686</v>
       </c>
       <c r="E12" s="12">
@@ -30291,7 +30966,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="40">
         <v>23175</v>
       </c>
       <c r="E13" s="12">
@@ -30339,7 +31014,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="40">
         <v>21204</v>
       </c>
       <c r="E14" s="12">
@@ -30390,7 +31065,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="40">
         <v>101365</v>
       </c>
       <c r="E15" s="12">
@@ -30439,7 +31114,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="40">
         <v>59057</v>
       </c>
       <c r="E16" s="12">
@@ -30487,7 +31162,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>22</v>
       </c>
-      <c r="D17" s="41">
+      <c r="D17" s="40">
         <v>119001</v>
       </c>
       <c r="E17" s="12">
@@ -30547,7 +31222,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="40">
         <v>36052</v>
       </c>
       <c r="E18" s="12">
@@ -30574,7 +31249,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="40">
         <v>73102</v>
       </c>
       <c r="E19" s="12">
@@ -30601,7 +31276,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="40">
         <v>23128</v>
       </c>
       <c r="E20" s="12">
@@ -30629,7 +31304,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="40">
         <v>79262</v>
       </c>
       <c r="E21" s="12">
@@ -30656,7 +31331,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="40">
         <v>116549</v>
       </c>
       <c r="E22" s="12">
@@ -30684,7 +31359,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="40">
         <v>86756</v>
       </c>
       <c r="E23" s="12">
@@ -30710,7 +31385,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
-      <c r="D24" s="41">
+      <c r="D24" s="40">
         <v>74666</v>
       </c>
       <c r="E24" s="12">
@@ -30738,7 +31413,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="40">
         <v>68347</v>
       </c>
       <c r="E25" s="12">
@@ -30766,7 +31441,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D26" s="41">
+      <c r="D26" s="40">
         <v>78409</v>
       </c>
       <c r="E26" s="12">
@@ -30791,7 +31466,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="40">
         <v>27853</v>
       </c>
       <c r="E27" s="12">
@@ -30816,7 +31491,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D28" s="41">
+      <c r="D28" s="40">
         <v>31037</v>
       </c>
       <c r="E28" s="12">
@@ -30841,7 +31516,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="40">
         <v>110448</v>
       </c>
       <c r="E29" s="12">
@@ -30868,7 +31543,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="40">
         <v>22189</v>
       </c>
       <c r="E30" s="12">
@@ -30895,7 +31570,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="40">
         <v>110203</v>
       </c>
       <c r="E31" s="12">
@@ -30922,7 +31597,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="D32" s="41">
+      <c r="D32" s="40">
         <v>101128</v>
       </c>
       <c r="E32" s="12">
@@ -30949,7 +31624,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
-      <c r="D33" s="41">
+      <c r="D33" s="40">
         <v>25849</v>
       </c>
       <c r="E33" s="12">
@@ -30976,7 +31651,7 @@
         <f t="shared" ref="C34:C65" ca="1" si="4">DATEDIF(B34,TODAY(),"Y")</f>
         <v>15</v>
       </c>
-      <c r="D34" s="41">
+      <c r="D34" s="40">
         <v>30049</v>
       </c>
       <c r="E34" s="12">
@@ -31003,7 +31678,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="D35" s="41">
+      <c r="D35" s="40">
         <v>96418</v>
       </c>
       <c r="E35" s="12">
@@ -31030,7 +31705,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>14</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D36" s="40">
         <v>121308</v>
       </c>
       <c r="E36" s="12">
@@ -31057,7 +31732,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>17</v>
       </c>
-      <c r="D37" s="41">
+      <c r="D37" s="40">
         <v>80732</v>
       </c>
       <c r="E37" s="12">
@@ -31084,7 +31759,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>14</v>
       </c>
-      <c r="D38" s="41">
+      <c r="D38" s="40">
         <v>27447</v>
       </c>
       <c r="E38" s="12">
@@ -31109,7 +31784,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>11</v>
       </c>
-      <c r="D39" s="41">
+      <c r="D39" s="40">
         <v>25015</v>
       </c>
       <c r="E39" s="12">
@@ -31136,7 +31811,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="D40" s="41">
+      <c r="D40" s="40">
         <v>59275</v>
       </c>
       <c r="E40" s="12">
@@ -31161,7 +31836,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>10</v>
       </c>
-      <c r="D41" s="41">
+      <c r="D41" s="40">
         <v>66573</v>
       </c>
       <c r="E41" s="12">
@@ -31188,7 +31863,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>14</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D42" s="40">
         <v>107695</v>
       </c>
       <c r="E42" s="12">
@@ -31213,7 +31888,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="D43" s="41">
+      <c r="D43" s="40">
         <v>115240</v>
       </c>
       <c r="E43" s="12">
@@ -31240,7 +31915,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D44" s="41">
+      <c r="D44" s="40">
         <v>27020</v>
       </c>
       <c r="E44" s="12">
@@ -31267,7 +31942,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="D45" s="41">
+      <c r="D45" s="40">
         <v>32375</v>
       </c>
       <c r="E45" s="12">
@@ -31292,7 +31967,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>14</v>
       </c>
-      <c r="D46" s="41">
+      <c r="D46" s="40">
         <v>75425</v>
       </c>
       <c r="E46" s="12">
@@ -31317,7 +31992,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D47" s="41">
+      <c r="D47" s="40">
         <v>26153</v>
       </c>
       <c r="E47" s="12">
@@ -31344,7 +32019,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="D48" s="41">
+      <c r="D48" s="40">
         <v>120404</v>
       </c>
       <c r="E48" s="12">
@@ -31369,7 +32044,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D49" s="41">
+      <c r="D49" s="40">
         <v>103608</v>
       </c>
       <c r="E49" s="12">
@@ -31396,7 +32071,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D50" s="41">
+      <c r="D50" s="40">
         <v>40917</v>
       </c>
       <c r="E50" s="12">
@@ -31423,7 +32098,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D51" s="41">
+      <c r="D51" s="40">
         <v>99457</v>
       </c>
       <c r="E51" s="12">
@@ -31450,7 +32125,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>14</v>
       </c>
-      <c r="D52" s="41">
+      <c r="D52" s="40">
         <v>27705</v>
       </c>
       <c r="E52" s="12">
@@ -31477,7 +32152,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>12</v>
       </c>
-      <c r="D53" s="41">
+      <c r="D53" s="40">
         <v>103657</v>
       </c>
       <c r="E53" s="12">
@@ -31504,7 +32179,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D54" s="41">
+      <c r="D54" s="40">
         <v>103259</v>
       </c>
       <c r="E54" s="12">
@@ -31531,7 +32206,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>12</v>
       </c>
-      <c r="D55" s="41">
+      <c r="D55" s="40">
         <v>84107</v>
       </c>
       <c r="E55" s="12">
@@ -31556,9 +32231,9 @@
       </c>
       <c r="C56" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="D56" s="41">
+        <v>14</v>
+      </c>
+      <c r="D56" s="40">
         <v>101481</v>
       </c>
       <c r="E56" s="12">
@@ -31585,7 +32260,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="D57" s="41">
+      <c r="D57" s="40">
         <v>44938</v>
       </c>
       <c r="E57" s="12">
@@ -31612,7 +32287,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D58" s="41">
+      <c r="D58" s="40">
         <v>70695</v>
       </c>
       <c r="E58" s="12">
@@ -31637,7 +32312,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>12</v>
       </c>
-      <c r="D59" s="41">
+      <c r="D59" s="40">
         <v>89510</v>
       </c>
       <c r="E59" s="12">
@@ -31662,7 +32337,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D60" s="41">
+      <c r="D60" s="40">
         <v>31323</v>
       </c>
       <c r="E60" s="12">
@@ -31689,7 +32364,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>7</v>
       </c>
-      <c r="D61" s="41">
+      <c r="D61" s="40">
         <v>51077</v>
       </c>
       <c r="E61" s="12">
@@ -31714,7 +32389,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D62" s="41">
+      <c r="D62" s="40">
         <v>72484</v>
       </c>
       <c r="E62" s="12">
@@ -31741,7 +32416,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D63" s="41">
+      <c r="D63" s="40">
         <v>48847</v>
       </c>
       <c r="E63" s="12">
@@ -31768,7 +32443,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="D64" s="41">
+      <c r="D64" s="40">
         <v>21737</v>
       </c>
       <c r="E64" s="12">
@@ -31795,7 +32470,7 @@
         <f t="shared" ca="1" si="4"/>
         <v>12</v>
       </c>
-      <c r="D65" s="41">
+      <c r="D65" s="40">
         <v>26463</v>
       </c>
       <c r="E65" s="12">
@@ -31822,7 +32497,7 @@
         <f t="shared" ref="C66:C97" ca="1" si="6">DATEDIF(B66,TODAY(),"Y")</f>
         <v>15</v>
       </c>
-      <c r="D66" s="41">
+      <c r="D66" s="40">
         <v>24870</v>
       </c>
       <c r="E66" s="12">
@@ -31849,7 +32524,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>10</v>
       </c>
-      <c r="D67" s="41">
+      <c r="D67" s="40">
         <v>66777</v>
       </c>
       <c r="E67" s="12">
@@ -31876,7 +32551,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>12</v>
       </c>
-      <c r="D68" s="41">
+      <c r="D68" s="40">
         <v>56571</v>
       </c>
       <c r="E68" s="12">
@@ -31903,7 +32578,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="D69" s="41">
+      <c r="D69" s="40">
         <v>42667</v>
       </c>
       <c r="E69" s="12">
@@ -31930,7 +32605,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>13</v>
       </c>
-      <c r="D70" s="41">
+      <c r="D70" s="40">
         <v>102833</v>
       </c>
       <c r="E70" s="12">
@@ -31957,7 +32632,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="D71" s="41">
+      <c r="D71" s="40">
         <v>26550</v>
       </c>
       <c r="E71" s="12">
@@ -31982,7 +32657,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="D72" s="41">
+      <c r="D72" s="40">
         <v>63477</v>
       </c>
       <c r="E72" s="12">
@@ -32009,7 +32684,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="D73" s="41">
+      <c r="D73" s="40">
         <v>27529</v>
       </c>
       <c r="E73" s="12">
@@ -32034,7 +32709,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>10</v>
       </c>
-      <c r="D74" s="41">
+      <c r="D74" s="40">
         <v>26272</v>
       </c>
       <c r="E74" s="12">
@@ -32061,7 +32736,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="D75" s="41">
+      <c r="D75" s="40">
         <v>23675</v>
       </c>
       <c r="E75" s="12">
@@ -32086,7 +32761,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>11</v>
       </c>
-      <c r="D76" s="41">
+      <c r="D76" s="40">
         <v>46201</v>
       </c>
       <c r="E76" s="12">
@@ -32113,7 +32788,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>8</v>
       </c>
-      <c r="D77" s="41">
+      <c r="D77" s="40">
         <v>23784</v>
       </c>
       <c r="E77" s="12">
@@ -32138,7 +32813,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>8</v>
       </c>
-      <c r="D78" s="41">
+      <c r="D78" s="40">
         <v>52956</v>
       </c>
       <c r="E78" s="12">
@@ -32165,7 +32840,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>11</v>
       </c>
-      <c r="D79" s="41">
+      <c r="D79" s="40">
         <v>23157</v>
       </c>
       <c r="E79" s="12">
@@ -32192,7 +32867,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="D80" s="41">
+      <c r="D80" s="40">
         <v>27006</v>
       </c>
       <c r="E80" s="12">
@@ -32219,7 +32894,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="D81" s="41">
+      <c r="D81" s="40">
         <v>110404</v>
       </c>
       <c r="E81" s="12">
@@ -32246,7 +32921,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="D82" s="41">
+      <c r="D82" s="40">
         <v>93239</v>
       </c>
       <c r="E82" s="12">
@@ -32271,7 +32946,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
-      <c r="D83" s="41">
+      <c r="D83" s="40">
         <v>39576</v>
       </c>
       <c r="E83" s="12">
@@ -32298,7 +32973,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="D84" s="41">
+      <c r="D84" s="40">
         <v>103041</v>
       </c>
       <c r="E84" s="12">
@@ -32325,7 +33000,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
-      <c r="D85" s="41">
+      <c r="D85" s="40">
         <v>119300</v>
       </c>
       <c r="E85" s="12">
@@ -32352,7 +33027,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="D86" s="41">
+      <c r="D86" s="40">
         <v>66579</v>
       </c>
       <c r="E86" s="12">
@@ -32379,7 +33054,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>13</v>
       </c>
-      <c r="D87" s="41">
+      <c r="D87" s="40">
         <v>110812</v>
       </c>
       <c r="E87" s="12">
@@ -32406,7 +33081,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>5</v>
       </c>
-      <c r="D88" s="41">
+      <c r="D88" s="40">
         <v>62335</v>
       </c>
       <c r="E88" s="12">
@@ -32431,7 +33106,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>12</v>
       </c>
-      <c r="D89" s="41">
+      <c r="D89" s="40">
         <v>98598</v>
       </c>
       <c r="E89" s="12">
@@ -32458,7 +33133,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="D90" s="41">
+      <c r="D90" s="40">
         <v>90126</v>
       </c>
       <c r="E90" s="12">
@@ -32485,7 +33160,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="D91" s="41">
+      <c r="D91" s="40">
         <v>71445</v>
       </c>
       <c r="E91" s="12">
@@ -32510,7 +33185,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="D92" s="41">
+      <c r="D92" s="40">
         <v>49419</v>
       </c>
       <c r="E92" s="12">
@@ -32535,7 +33210,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="D93" s="41">
+      <c r="D93" s="40">
         <v>55819</v>
       </c>
       <c r="E93" s="12">
@@ -32562,7 +33237,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>8</v>
       </c>
-      <c r="D94" s="41">
+      <c r="D94" s="40">
         <v>60730</v>
       </c>
       <c r="E94" s="12">
@@ -32589,7 +33264,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="D95" s="41">
+      <c r="D95" s="40">
         <v>119949</v>
       </c>
       <c r="E95" s="12">
@@ -32616,7 +33291,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="D96" s="41">
+      <c r="D96" s="40">
         <v>83926</v>
       </c>
       <c r="E96" s="12">
@@ -32641,7 +33316,7 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="D97" s="41">
+      <c r="D97" s="40">
         <v>114408</v>
       </c>
       <c r="E97" s="12">
@@ -32668,7 +33343,7 @@
         <f ca="1">DATEDIF(B98,TODAY(),"Y")</f>
         <v>2</v>
       </c>
-      <c r="D98" s="41">
+      <c r="D98" s="40">
         <v>113020</v>
       </c>
       <c r="E98" s="12">
@@ -32695,7 +33370,7 @@
         <f ca="1">DATEDIF(B99,TODAY(),"Y")</f>
         <v>1</v>
       </c>
-      <c r="D99" s="41">
+      <c r="D99" s="40">
         <v>121824</v>
       </c>
       <c r="E99" s="12">
@@ -32722,7 +33397,7 @@
         <f ca="1">DATEDIF(B100,TODAY(),"Y")</f>
         <v>1</v>
       </c>
-      <c r="D100" s="41">
+      <c r="D100" s="40">
         <v>21697</v>
       </c>
       <c r="E100" s="12">
@@ -36618,6 +37293,9 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -36629,7 +37307,9 @@
   </sheetPr>
   <dimension ref="A1:I742"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -36639,7 +37319,7 @@
     <col min="4" max="4" width="15.21875" style="30" customWidth="1"/>
     <col min="5" max="5" width="18.88671875" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" style="3"/>
     <col min="9" max="16384" width="19.88671875" style="4"/>
   </cols>
@@ -36658,13 +37338,13 @@
         <v>830</v>
       </c>
       <c r="E1" s="29"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>823</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>824</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="44" t="s">
         <v>827</v>
       </c>
     </row>
@@ -36747,6 +37427,13 @@
       <c r="C5" s="12">
         <v>39604</v>
       </c>
+      <c r="F5" s="3">
+        <f>COUNT(C:C)</f>
+        <v>99</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -36760,6 +37447,13 @@
       </c>
       <c r="D6" s="30">
         <v>6</v>
+      </c>
+      <c r="F6" s="3">
+        <f>COUNTA(C:C)</f>
+        <v>100</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>